<commit_message>
feat[catalogue]: simplified data model while accomodating more depth for cohorts
</commit_message>
<xml_diff>
--- a/data/datacatalogue/Conception.xlsx
+++ b/data/datacatalogue/Conception.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/data/datacatalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB0F770-A6EF-DD4D-9A7D-97F963BD6763}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3F668D-6653-2446-9050-8C532E8B45FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="20500" firstSheet="28" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Institutions" sheetId="23" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8884" uniqueCount="2512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8884" uniqueCount="2514">
   <si>
     <t>description</t>
   </si>
@@ -7722,6 +7722,12 @@
   </si>
   <si>
     <t>GCC,EUROCAT</t>
+  </si>
+  <si>
+    <t>fundingDescription</t>
+  </si>
+  <si>
+    <t>fundingStatement</t>
   </si>
 </sst>
 </file>
@@ -12481,7 +12487,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12534,8 +12542,8 @@
       <c r="M1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>61</v>
+      <c r="N1" s="13" t="s">
+        <v>2512</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>62</v>
@@ -14270,11 +14278,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:Y22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="H19" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
+      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14342,7 +14350,7 @@
         <v>2505</v>
       </c>
       <c r="O1" s="13" t="s">
-        <v>61</v>
+        <v>2512</v>
       </c>
       <c r="P1" s="13" t="s">
         <v>62</v>
@@ -15442,7 +15450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -27738,13 +27746,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="95" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
@@ -27788,7 +27797,7 @@
         <v>60</v>
       </c>
       <c r="N1" t="s">
-        <v>61</v>
+        <v>2513</v>
       </c>
       <c r="O1" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
Revert "Add feature to have 'draft' and have insertedBy / modifiedBy metadata information"
</commit_message>
<xml_diff>
--- a/data/datacatalogue/Conception.xlsx
+++ b/data/datacatalogue/Conception.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/data/datacatalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3F668D-6653-2446-9050-8C532E8B45FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB0F770-A6EF-DD4D-9A7D-97F963BD6763}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="20500" firstSheet="28" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Institutions" sheetId="23" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8884" uniqueCount="2514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8884" uniqueCount="2512">
   <si>
     <t>description</t>
   </si>
@@ -7722,12 +7722,6 @@
   </si>
   <si>
     <t>GCC,EUROCAT</t>
-  </si>
-  <si>
-    <t>fundingDescription</t>
-  </si>
-  <si>
-    <t>fundingStatement</t>
   </si>
 </sst>
 </file>
@@ -12487,9 +12481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12542,8 +12534,8 @@
       <c r="M1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="N1" s="13" t="s">
-        <v>2512</v>
+      <c r="N1" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>62</v>
@@ -14278,11 +14270,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:Y22"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="H19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
+      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14350,7 +14342,7 @@
         <v>2505</v>
       </c>
       <c r="O1" s="13" t="s">
-        <v>2512</v>
+        <v>61</v>
       </c>
       <c r="P1" s="13" t="s">
         <v>62</v>
@@ -15450,7 +15442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -27746,14 +27738,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="95" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
@@ -27797,7 +27788,7 @@
         <v>60</v>
       </c>
       <c r="N1" t="s">
-        <v>2513</v>
+        <v>61</v>
       </c>
       <c r="O1" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
Revert "Revert "Add feature to have 'draft' and have insertedBy / modifiedBy metadata information""
</commit_message>
<xml_diff>
--- a/data/datacatalogue/Conception.xlsx
+++ b/data/datacatalogue/Conception.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/data/datacatalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB0F770-A6EF-DD4D-9A7D-97F963BD6763}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3F668D-6653-2446-9050-8C532E8B45FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="20500" firstSheet="28" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Institutions" sheetId="23" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8884" uniqueCount="2512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8884" uniqueCount="2514">
   <si>
     <t>description</t>
   </si>
@@ -7722,6 +7722,12 @@
   </si>
   <si>
     <t>GCC,EUROCAT</t>
+  </si>
+  <si>
+    <t>fundingDescription</t>
+  </si>
+  <si>
+    <t>fundingStatement</t>
   </si>
 </sst>
 </file>
@@ -12481,7 +12487,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12534,8 +12542,8 @@
       <c r="M1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>61</v>
+      <c r="N1" s="13" t="s">
+        <v>2512</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>62</v>
@@ -14270,11 +14278,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:Y22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="H19" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
+      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14342,7 +14350,7 @@
         <v>2505</v>
       </c>
       <c r="O1" s="13" t="s">
-        <v>61</v>
+        <v>2512</v>
       </c>
       <c r="P1" s="13" t="s">
         <v>62</v>
@@ -15442,7 +15450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -27738,13 +27746,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="95" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
@@ -27788,7 +27797,7 @@
         <v>60</v>
       </c>
       <c r="N1" t="s">
-        <v>61</v>
+        <v>2513</v>
       </c>
       <c r="O1" t="s">
         <v>62</v>

</xml_diff>